<commit_message>
minor mistypping fixed in Fix_tests.xlsx
</commit_message>
<xml_diff>
--- a/Fix_tests.xlsx
+++ b/Fix_tests.xlsx
@@ -39,9 +39,6 @@
     <t>Открыть адресс: http://rulkov.ru/qa</t>
   </si>
   <si>
-    <t>Клик на 'Операция сложения' линка</t>
-  </si>
-  <si>
     <t>Ввести 3 корректных числа</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>Ввести 3 корректных числа результат сложения которых будет четное число.</t>
   </si>
   <si>
-    <t>Ввести 3 корректных числа результат хотя бы  одно из которых больше 2e+1023</t>
-  </si>
-  <si>
     <t>Нажать на линк 'Logout'</t>
   </si>
   <si>
@@ -211,6 +205,12 @@
   </si>
   <si>
     <t>н/а</t>
+  </si>
+  <si>
+    <t>Ввести 3 корректных числа хотя бы  одно из которых больше 2e+1023</t>
+  </si>
+  <si>
+    <t>Клик на линк 'Операция сложения'</t>
   </si>
 </sst>
 </file>
@@ -400,6 +400,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -409,6 +424,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -416,24 +434,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11:H13"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28:F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -754,71 +754,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="32.25" customHeight="1">
-      <c r="A1" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="18" t="s">
+      <c r="A1" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="16"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="20"/>
+    </row>
+    <row r="3" spans="1:9" hidden="1">
+      <c r="A3" s="16">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="18"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="22"/>
-    </row>
-    <row r="3" spans="1:9" hidden="1">
-      <c r="A3" s="18">
-        <v>1</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>58</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="18">
+      <c r="F3" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="16">
         <v>5</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="16">
         <v>1</v>
       </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="18"/>
-      <c r="B4" s="22"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="9">
         <v>1</v>
       </c>
@@ -826,55 +826,55 @@
         <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
+        <v>15</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="30">
-      <c r="A5" s="18"/>
-      <c r="B5" s="22"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="9">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
+        <v>17</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="60">
-      <c r="A6" s="18"/>
-      <c r="B6" s="22"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="9">
         <v>3</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
+        <v>23</v>
+      </c>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
       <c r="I6" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="18">
+      <c r="A7" s="16">
         <v>2</v>
       </c>
-      <c r="B7" s="22" t="s">
-        <v>52</v>
+      <c r="B7" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="C7" s="9">
         <v>1</v>
@@ -883,70 +883,70 @@
         <v>6</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="18">
+        <v>15</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="16">
         <v>5</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="16">
         <v>1</v>
       </c>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="30">
-      <c r="A8" s="18"/>
-      <c r="B8" s="22"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="9">
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
+        <v>17</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="60">
-      <c r="A9" s="18"/>
-      <c r="B9" s="22"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="9">
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
+        <v>52</v>
+      </c>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" hidden="1">
       <c r="A10" s="9"/>
-      <c r="B10" s="23"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="9"/>
       <c r="D10" s="2"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="12">
+      <c r="A11" s="17">
         <v>3</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>60</v>
+      <c r="B11" s="23" t="s">
+        <v>58</v>
       </c>
       <c r="C11" s="9">
         <v>1</v>
@@ -955,73 +955,73 @@
         <v>6</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>64</v>
+        <v>15</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30">
-      <c r="A12" s="13"/>
-      <c r="B12" s="15"/>
+      <c r="A12" s="18"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="9">
         <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
+        <v>17</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="18"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="45">
-      <c r="A13" s="14"/>
-      <c r="B13" s="16"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="9">
         <v>3</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
+        <v>61</v>
+      </c>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" ht="30">
       <c r="A14" s="9">
         <v>4</v>
       </c>
-      <c r="B14" s="23" t="s">
-        <v>48</v>
+      <c r="B14" s="15" t="s">
+        <v>46</v>
       </c>
       <c r="C14" s="9">
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G14" s="9">
         <v>1</v>
@@ -1032,365 +1032,365 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" ht="259.5" customHeight="1">
-      <c r="A15" s="13">
+      <c r="A15" s="18">
         <v>5</v>
       </c>
-      <c r="B15" s="15" t="s">
-        <v>45</v>
+      <c r="B15" s="21" t="s">
+        <v>43</v>
       </c>
       <c r="C15" s="7">
         <v>1</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" s="13">
+      <c r="D15" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="18">
         <v>30</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="18">
         <v>26</v>
       </c>
-      <c r="I15" s="21" t="s">
-        <v>36</v>
+      <c r="I15" s="14" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30">
-      <c r="A16" s="13"/>
-      <c r="B16" s="15"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="8">
         <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+        <v>19</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
       <c r="I16" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="120">
-      <c r="A17" s="13"/>
-      <c r="B17" s="15"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="21"/>
       <c r="C17" s="8">
         <v>3</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+        <v>21</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
       <c r="I17" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30">
-      <c r="A18" s="13"/>
-      <c r="B18" s="15"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="21"/>
       <c r="C18" s="8">
         <v>4</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+        <v>24</v>
+      </c>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" ht="30">
-      <c r="A19" s="14"/>
-      <c r="B19" s="16"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="22"/>
       <c r="C19" s="8">
         <v>5</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
+        <v>25</v>
+      </c>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" hidden="1">
-      <c r="A20" s="12">
+      <c r="A20" s="17">
         <v>6</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="23" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="H20" s="18" t="s">
-        <v>64</v>
+      <c r="F20" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>62</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="30">
-      <c r="A21" s="13"/>
-      <c r="B21" s="15"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="8">
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
+        <v>26</v>
+      </c>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
       <c r="I21" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45">
-      <c r="A22" s="13"/>
-      <c r="B22" s="15"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="21"/>
       <c r="C22" s="8">
         <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="13"/>
-      <c r="B23" s="15"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="21"/>
       <c r="C23" s="8">
         <v>3</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
+        <v>24</v>
+      </c>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" ht="30">
-      <c r="A24" s="14"/>
-      <c r="B24" s="16"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="22"/>
       <c r="C24" s="8">
         <v>4</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
+        <v>27</v>
+      </c>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
       <c r="I24" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="13">
+      <c r="A25" s="18">
         <v>7</v>
       </c>
-      <c r="B25" s="15" t="s">
-        <v>46</v>
+      <c r="B25" s="21" t="s">
+        <v>44</v>
       </c>
       <c r="C25" s="8">
         <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F25" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="G25" s="18">
+      <c r="F25" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="16">
         <v>5</v>
       </c>
-      <c r="H25" s="18">
+      <c r="H25" s="16">
         <v>4</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="30">
-      <c r="A26" s="13"/>
-      <c r="B26" s="15"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="21"/>
       <c r="C26" s="8">
         <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
+        <v>19</v>
+      </c>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9" ht="150">
-      <c r="A27" s="14"/>
-      <c r="B27" s="16"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="22"/>
       <c r="C27" s="8">
         <v>3</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
+        <v>28</v>
+      </c>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
       <c r="I27" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="30">
-      <c r="A28" s="13">
+      <c r="A28" s="18">
         <v>8</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>47</v>
+      <c r="B28" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="C28" s="8">
         <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G28" s="13">
+      <c r="F28" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="18">
         <v>5</v>
       </c>
-      <c r="H28" s="13">
+      <c r="H28" s="18">
         <v>8</v>
       </c>
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9" ht="30">
-      <c r="A29" s="13"/>
-      <c r="B29" s="15"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="8">
         <v>2</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+        <v>19</v>
+      </c>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:9" ht="120">
-      <c r="A30" s="14"/>
-      <c r="B30" s="16"/>
+      <c r="A30" s="19"/>
+      <c r="B30" s="22"/>
       <c r="C30" s="8">
         <v>3</v>
       </c>
       <c r="D30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" hidden="1">
+      <c r="A31" s="17">
         <v>9</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" hidden="1">
-      <c r="A31" s="12">
-        <v>9</v>
-      </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G31" s="12">
+      <c r="F31" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="17">
         <v>1</v>
       </c>
-      <c r="H31" s="12">
+      <c r="H31" s="17">
         <v>0.5</v>
       </c>
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9" ht="30">
-      <c r="A32" s="14"/>
-      <c r="B32" s="16"/>
+      <c r="A32" s="19"/>
+      <c r="B32" s="22"/>
       <c r="C32" s="8">
         <v>1</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
+        <v>33</v>
+      </c>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
       <c r="I32" s="2"/>
     </row>
     <row r="34" spans="1:1">
@@ -1400,18 +1400,26 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="G7:G10"/>
-    <mergeCell ref="H7:H10"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="H28:H30"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G3:G6"/>
-    <mergeCell ref="H3:H6"/>
-    <mergeCell ref="G15:G19"/>
-    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="F3:F6"/>
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="F25:F27"/>
     <mergeCell ref="F28:F30"/>
     <mergeCell ref="G31:G32"/>
     <mergeCell ref="H31:H32"/>
@@ -1428,26 +1436,18 @@
     <mergeCell ref="G25:G27"/>
     <mergeCell ref="H25:H27"/>
     <mergeCell ref="G28:G30"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="F3:F6"/>
-    <mergeCell ref="F15:F19"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="A25:A27"/>
-    <mergeCell ref="A3:A6"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="H28:H30"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G3:G6"/>
+    <mergeCell ref="H3:H6"/>
+    <mergeCell ref="G15:G19"/>
+    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="H11:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>